<commit_message>
HRM New Candidate Adding Steps
</commit_message>
<xml_diff>
--- a/Data/Employee List.xlsx
+++ b/Data/Employee List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prathap.tadi\Documents\UiPath\TestAutomationFramework_HRM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D448593-3F4C-4E1B-9910-525169354484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA0FDDE-5062-4A4D-B133-D36847241A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Test123</t>
   </si>
   <si>
     <t>UserRole</t>
@@ -943,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,22 +965,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -997,7 +975,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,28 +992,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1046,22 +1024,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>